<commit_message>
began working on UI
</commit_message>
<xml_diff>
--- a/ExcelDemo.xlsx
+++ b/ExcelDemo.xlsx
@@ -55,12 +55,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>